<commit_message>
considered table constitution roughly
</commit_message>
<xml_diff>
--- a/UI/バスケットゴールアプリ_設計.xlsx
+++ b/UI/バスケットゴールアプリ_設計.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keita\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keita\Documents\GitHub\basketgoal_app\UI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151B409D-E276-42E2-A53E-8FB84760EC3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC24A44-290E-4A35-B340-73699534F673}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{1927E6A8-C1F1-4097-884E-FA9E92B27A77}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="1" xr2:uid="{1927E6A8-C1F1-4097-884E-FA9E92B27A77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="153">
   <si>
     <t>リクエスト内容</t>
     <rPh sb="5" eb="7">
@@ -118,40 +119,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/user/</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>(1) ユーザー管理  user</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>(2) ゴール管理  goal</t>
-    <rPh sb="7" eb="9">
-      <t>カンリ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>(3) 場所管理 place</t>
-    <rPh sb="4" eb="6">
-      <t>バショ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>カンリ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/goal/</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/place/</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -212,16 +180,6 @@
   </si>
   <si>
     <t>ユーザー更新画面</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>(4) 画面遷移アプリ</t>
-    <rPh sb="4" eb="6">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>センイ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1018,12 +976,388 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>(1) ユーザー管理  manageuser</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/manageuser/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/managegoal/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/manageplace/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(2) ゴール管理  managegoal</t>
+    <rPh sb="7" eb="9">
+      <t>カンリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(3) 場所管理 manageplace</t>
+    <rPh sb="4" eb="6">
+      <t>バショ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>カンリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(4) 画面遷移アプリ transition</t>
+    <rPh sb="4" eb="6">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>センイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>モデルの設計</t>
+    <rPh sb="4" eb="6">
+      <t>セッケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>user</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pk</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>主キー(自動で作成)</t>
+    <rPh sb="0" eb="1">
+      <t>シュ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ジドウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>サクセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>名前</t>
+    <rPh sb="0" eb="2">
+      <t>ナマエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>password</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パスワード</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>image</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アイコン画像</t>
+    <rPh sb="4" eb="6">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>備考</t>
+    <rPh sb="0" eb="2">
+      <t>ビコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>変数</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>説明</t>
+    <rPh sb="0" eb="2">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>goal</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>address</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>住所</t>
+    <rPh sb="0" eb="2">
+      <t>ジュウショ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ゴールの場所</t>
+    <rPh sb="4" eb="6">
+      <t>バショ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ゴールの画像</t>
+    <rPh sb="4" eb="6">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>starttime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>endtime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>利用可能開始時間</t>
+    <rPh sb="0" eb="2">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ジカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>利用可能終了時間</t>
+    <rPh sb="0" eb="2">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>シュウリョウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ジカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ホームページなどのURL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>explanation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>otherinfo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>place</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>県名</t>
+    <rPh sb="0" eb="2">
+      <t>ケンメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>placepk</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>placeの主キー(外部キー)</t>
+    <rPh sb="6" eb="7">
+      <t>シュ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ガイブ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>userpk</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>impression</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>goalpk</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ゴールの主キー(外部キー)</t>
+    <rPh sb="4" eb="5">
+      <t>シュ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ガイブ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>感想を記載したユーザーの主キー(外部キー)</t>
+    <rPh sb="0" eb="2">
+      <t>カンソウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>キサイ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>シュ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ガイブ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>感想</t>
+    <rPh sb="0" eb="2">
+      <t>カンソウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>changedvariable</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>変更した変数</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>before</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>changedvariableで指定した変数の前の状態</t>
+    <rPh sb="16" eb="18">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ジョウタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>after</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>changedvariableで指定した変数の後の状態</t>
+    <rPh sb="16" eb="18">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ジョウタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>good</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>変更に対してのいいね</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>タイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>changedhistory</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>changeapplication</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>データ型</t>
+    <rPh sb="3" eb="4">
+      <t>ガタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>integer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>いいね</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1036,6 +1370,14 @@
       <sz val="6"/>
       <name val="游ゴシック"/>
       <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -1054,7 +1396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1091,13 +1433,265 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1121,6 +1715,84 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1438,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123A1A13-25A3-429B-A121-0002F32709A3}">
   <dimension ref="A1:AA125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A13" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1547,10 +2219,10 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1"/>
       <c r="I4" s="1"/>
@@ -1577,10 +2249,10 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1"/>
       <c r="I5" s="1"/>
@@ -1606,10 +2278,10 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1634,13 +2306,13 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1695,7 +2367,7 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1736,13 +2408,13 @@
         <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1777,10 +2449,10 @@
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H11" s="1">
         <v>18</v>
@@ -1818,10 +2490,10 @@
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H12" s="1">
         <v>20</v>
@@ -1859,13 +2531,13 @@
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1900,10 +2572,10 @@
         <v>12</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H14" s="1">
         <v>12</v>
@@ -1932,19 +2604,19 @@
       <c r="A15" s="2"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1999,7 +2671,7 @@
     <row r="17" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2040,13 +2712,13 @@
         <v>1</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2072,19 +2744,19 @@
       <c r="A19" s="2"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H19" s="1">
         <v>14</v>
@@ -2113,19 +2785,19 @@
       <c r="A20" s="2"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="H20" s="1">
         <v>22</v>
@@ -2154,19 +2826,19 @@
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H21" s="1">
         <v>10</v>
@@ -2195,19 +2867,19 @@
       <c r="A22" s="2"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H22" s="1">
         <v>7</v>
@@ -2234,19 +2906,19 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.4">
       <c r="C23" s="6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="H23" s="6">
         <v>15</v>
@@ -2295,7 +2967,7 @@
     <row r="25" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2336,13 +3008,13 @@
         <v>1</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -2368,19 +3040,19 @@
       <c r="A27" s="2"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H27" s="1">
         <v>3</v>
@@ -2409,19 +3081,19 @@
       <c r="A28" s="2"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H28" s="1">
         <v>5</v>
@@ -2448,19 +3120,19 @@
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.4">
       <c r="C29" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E29" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="H29" s="1">
         <v>4</v>
@@ -2517,7 +3189,7 @@
     <row r="31" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2558,13 +3230,13 @@
         <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -2590,19 +3262,19 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H33" s="1">
         <v>1</v>
@@ -2631,7 +3303,7 @@
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>15</v>
@@ -2640,10 +3312,10 @@
         <v>14</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="H34" s="1">
         <v>2</v>
@@ -2672,22 +3344,22 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -2713,19 +3385,19 @@
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H36" s="1">
         <v>8</v>
@@ -2754,19 +3426,19 @@
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="H37" s="1">
         <v>9</v>
@@ -2795,22 +3467,22 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2836,19 +3508,19 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H39" s="1">
         <v>21</v>
@@ -2877,19 +3549,19 @@
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F40" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -5382,4 +6054,495 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0AC32C2-AC6A-4403-BE86-C6B7A5592E26}">
+  <dimension ref="C4:E57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="17.875" customWidth="1"/>
+    <col min="4" max="4" width="40.75" customWidth="1"/>
+    <col min="5" max="5" width="23.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C7" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C9" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C10" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C11" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C12" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C15" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="C16" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C17" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C18" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C19" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C20" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C21" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C22" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C23" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C24" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C25" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C28" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="C29" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C30" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="33" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C34" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="C35" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C36" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C37" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C38" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C39" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E39" s="33" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="41" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C42" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" s="26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="C43" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C44" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C45" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C46" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C47" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="49" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C49" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C50" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="C51" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E51" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C52" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C53" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C54" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E54" s="25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C55" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="E55" s="25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C56" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.4"/>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>